<commit_message>
neural network with 4 % of error
</commit_message>
<xml_diff>
--- a/neural networks/possibilidades quizz.xlsx
+++ b/neural networks/possibilidades quizz.xlsx
@@ -1,15 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A16E4E5A-3B0C-4A70-A156-D05D112EAAC8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -52,7 +61,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -89,17 +98,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -126,7 +125,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -164,7 +163,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -199,6 +198,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -234,9 +250,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -409,11 +442,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,10 +536,10 @@
         <v>-2</v>
       </c>
       <c r="C3" s="1">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="D3" s="1">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="E3" s="1">
         <v>-1</v>
@@ -521,8 +554,8 @@
         <v>-2</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I81" si="0">26+SUM(A3:H3)</f>
-        <v>9</v>
+        <f t="shared" ref="I3:I82" si="0">26+SUM(A3:H3)</f>
+        <v>11</v>
       </c>
       <c r="K3" t="str">
         <f t="shared" ref="K3:K66" si="1">IF(I3&lt;7,"0, 0, 0, 0, 1", IF(I3&lt;13,"0, 0, 0, 1, 0", IF(I3&lt;19,"0, 0, 1, 0, 0",IF(I3&lt;25,"0, 1, 0, 0, 0",IF(I3&lt;27,"1, 0, 0, 0, 0","")))))</f>
@@ -538,13 +571,13 @@
         <v>-3</v>
       </c>
       <c r="B4">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="C4">
         <v>-2</v>
       </c>
       <c r="D4">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E4">
         <v>-3</v>
@@ -567,7 +600,7 @@
         <v>0, 0, 0, 1, 0</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" ref="L3:L66" si="2">IF(SUMPRODUCT(($A$2:$A$81=A4)*1, ($B$2:$B$81=B4)*1, ($C$2:$C$81=C4)*1,($D$2:$D$81=D4)*1,($E$2:$E$81=E4)*1,($F$2:$F$81=F4)*1,($G$2:$G$81=G4)*1,($H$2:$H$81=H4)*1 ) &gt;1, "duplicates", "no duplicates")</f>
+        <f t="shared" ref="L4:L66" si="2">IF(SUMPRODUCT(($A$2:$A$81=A4)*1, ($B$2:$B$81=B4)*1, ($C$2:$C$81=C4)*1,($D$2:$D$81=D4)*1,($E$2:$E$81=E4)*1,($F$2:$F$81=F4)*1,($G$2:$G$81=G4)*1,($H$2:$H$81=H4)*1 ) &gt;1, "duplicates", "no duplicates")</f>
         <v>no duplicates</v>
       </c>
     </row>
@@ -582,7 +615,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>-2</v>
@@ -598,7 +631,7 @@
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="1"/>
@@ -620,7 +653,7 @@
         <v>-3</v>
       </c>
       <c r="D6">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -636,7 +669,7 @@
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="1"/>
@@ -655,7 +688,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="D7">
         <v>-2</v>
@@ -674,10 +707,10 @@
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(I7&lt;7,"0, 0, 0, 0, 1", IF(I7&lt;13,"0, 0, 0, 1, 0", IF(I7&lt;19,"0, 0, 1, 0, 0",IF(I7&lt;25,"0, 1, 0, 0, 0",IF(I7&lt;27,"1, 0, 0, 0, 0","")))))</f>
         <v>0, 0, 1, 0, 0</v>
       </c>
       <c r="L7" t="str">
@@ -696,7 +729,7 @@
         <v>-2</v>
       </c>
       <c r="D8">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="E8">
         <v>-3</v>
@@ -712,7 +745,7 @@
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="1"/>
@@ -810,10 +843,10 @@
         <v>-3</v>
       </c>
       <c r="D11">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -848,13 +881,13 @@
         <v>-3</v>
       </c>
       <c r="D12">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -924,13 +957,13 @@
         <v>-3</v>
       </c>
       <c r="D14">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E14">
         <v>-2</v>
       </c>
       <c r="F14">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="G14">
         <v>-2</v>
@@ -997,10 +1030,10 @@
         <v>-3</v>
       </c>
       <c r="C16">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="D16">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E16">
         <v>-3</v>
@@ -1009,14 +1042,14 @@
         <v>-3</v>
       </c>
       <c r="G16">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="H16">
         <v>-3</v>
       </c>
       <c r="I16">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="1"/>
@@ -1035,10 +1068,10 @@
         <v>-3</v>
       </c>
       <c r="C17">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="D17">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E17">
         <v>-3</v>
@@ -1054,7 +1087,7 @@
       </c>
       <c r="I17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K17" t="str">
         <f t="shared" si="1"/>
@@ -1076,7 +1109,7 @@
         <v>-2</v>
       </c>
       <c r="D18">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1092,7 +1125,7 @@
       </c>
       <c r="I18">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K18" t="str">
         <f t="shared" si="1"/>
@@ -1111,10 +1144,10 @@
         <v>-2</v>
       </c>
       <c r="C19">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="D19">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1130,7 +1163,7 @@
       </c>
       <c r="I19">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="K19" t="str">
         <f t="shared" si="1"/>
@@ -1149,10 +1182,10 @@
         <v>-3</v>
       </c>
       <c r="C20">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="D20">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="E20">
         <v>-1</v>
@@ -1228,13 +1261,13 @@
         <v>-2</v>
       </c>
       <c r="D22">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E22">
         <v>-3</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G22">
         <v>-2</v>
@@ -1304,7 +1337,7 @@
         <v>-1</v>
       </c>
       <c r="D24">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1320,7 +1353,7 @@
       </c>
       <c r="I24">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K24" t="str">
         <f t="shared" si="1"/>
@@ -1342,7 +1375,7 @@
         <v>-2</v>
       </c>
       <c r="D25">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="E25">
         <v>-2</v>
@@ -1358,7 +1391,7 @@
       </c>
       <c r="I25">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K25" t="str">
         <f t="shared" si="1"/>
@@ -1380,7 +1413,7 @@
         <v>-2</v>
       </c>
       <c r="D26">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1396,7 +1429,7 @@
       </c>
       <c r="I26">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" si="1"/>
@@ -1418,7 +1451,7 @@
         <v>-3</v>
       </c>
       <c r="D27">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E27">
         <v>-3</v>
@@ -1434,7 +1467,7 @@
       </c>
       <c r="I27">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K27" t="str">
         <f t="shared" si="1"/>
@@ -1456,10 +1489,10 @@
         <v>-2</v>
       </c>
       <c r="D28">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E28">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="F28">
         <v>-3</v>
@@ -1491,10 +1524,10 @@
         <v>-3</v>
       </c>
       <c r="C29">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="D29">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E29">
         <v>-1</v>
@@ -1510,7 +1543,7 @@
       </c>
       <c r="I29">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K29" t="str">
         <f t="shared" si="1"/>
@@ -1570,7 +1603,7 @@
         <v>-3</v>
       </c>
       <c r="D31">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E31">
         <v>-2</v>
@@ -1586,7 +1619,7 @@
       </c>
       <c r="I31">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K31" t="str">
         <f t="shared" si="1"/>
@@ -1605,7 +1638,7 @@
         <v>-2</v>
       </c>
       <c r="C32">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="D32">
         <v>-2</v>
@@ -1624,7 +1657,7 @@
       </c>
       <c r="I32">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K32" t="str">
         <f t="shared" si="1"/>
@@ -1684,13 +1717,13 @@
         <v>-1</v>
       </c>
       <c r="D34">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E34">
         <v>-2</v>
       </c>
       <c r="F34">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="G34">
         <v>-2</v>
@@ -1722,7 +1755,7 @@
         <v>-3</v>
       </c>
       <c r="D35">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E35">
         <v>-3</v>
@@ -1738,7 +1771,7 @@
       </c>
       <c r="I35">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K35" t="str">
         <f t="shared" si="1"/>
@@ -1798,7 +1831,7 @@
         <v>0</v>
       </c>
       <c r="D37">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="E37">
         <v>-1</v>
@@ -1813,8 +1846,8 @@
         <v>0</v>
       </c>
       <c r="I37">
-        <f t="shared" si="0"/>
-        <v>21</v>
+        <f>26+SUM(A37:H37)</f>
+        <v>22</v>
       </c>
       <c r="K37" t="str">
         <f t="shared" si="1"/>
@@ -1836,13 +1869,13 @@
         <v>-3</v>
       </c>
       <c r="D38">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E38">
         <v>-3</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G38">
         <v>-3</v>
@@ -1874,7 +1907,7 @@
         <v>-3</v>
       </c>
       <c r="D39">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E39">
         <v>-3</v>
@@ -1883,7 +1916,7 @@
         <v>-2</v>
       </c>
       <c r="G39">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="H39">
         <v>-3</v>
@@ -1912,7 +1945,7 @@
         <v>-2</v>
       </c>
       <c r="D40">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E40">
         <v>-2</v>
@@ -1928,7 +1961,7 @@
       </c>
       <c r="I40">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K40" t="str">
         <f t="shared" si="1"/>
@@ -1988,7 +2021,7 @@
         <v>0</v>
       </c>
       <c r="D42">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -2004,7 +2037,7 @@
       </c>
       <c r="I42">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K42" t="str">
         <f t="shared" si="1"/>
@@ -2064,7 +2097,7 @@
         <v>0</v>
       </c>
       <c r="D44">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -2080,7 +2113,7 @@
       </c>
       <c r="I44">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K44" t="str">
         <f t="shared" si="1"/>
@@ -2140,7 +2173,7 @@
         <v>0</v>
       </c>
       <c r="D46">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -2156,7 +2189,7 @@
       </c>
       <c r="I46">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K46" t="str">
         <f t="shared" si="1"/>
@@ -2254,7 +2287,7 @@
         <v>-3</v>
       </c>
       <c r="D49">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E49">
         <v>-2</v>
@@ -2270,7 +2303,7 @@
       </c>
       <c r="I49">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K49" t="str">
         <f t="shared" si="1"/>
@@ -2368,7 +2401,7 @@
         <v>-1</v>
       </c>
       <c r="D52">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="E52">
         <v>0</v>
@@ -2384,7 +2417,7 @@
       </c>
       <c r="I52">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K52" t="str">
         <f t="shared" si="1"/>
@@ -2406,10 +2439,10 @@
         <v>-3</v>
       </c>
       <c r="D53">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E53">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F53">
         <v>-1</v>
@@ -2815,7 +2848,7 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B64">
         <v>-3</v>
@@ -2824,10 +2857,10 @@
         <v>-3</v>
       </c>
       <c r="D64">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E64">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="F64">
         <v>-3</v>
@@ -2840,7 +2873,7 @@
       </c>
       <c r="I64">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K64" t="str">
         <f t="shared" si="1"/>
@@ -2853,16 +2886,16 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B65">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="C65">
         <v>-2</v>
       </c>
       <c r="D65">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E65">
         <v>-3</v>
@@ -2878,11 +2911,11 @@
       </c>
       <c r="I65">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K65" t="str">
         <f t="shared" si="1"/>
-        <v>0, 0, 0, 1, 0</v>
+        <v>0, 0, 0, 0, 1</v>
       </c>
       <c r="L65" t="str">
         <f t="shared" si="2"/>
@@ -2900,7 +2933,7 @@
         <v>-3</v>
       </c>
       <c r="D66">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E66">
         <v>-3</v>
@@ -2916,7 +2949,7 @@
       </c>
       <c r="I66">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K66" t="str">
         <f t="shared" si="1"/>
@@ -2957,11 +2990,11 @@
         <v>23</v>
       </c>
       <c r="K67" t="str">
-        <f t="shared" ref="K67:K81" si="3">IF(I67&lt;7,"0, 0, 0, 0, 1", IF(I67&lt;13,"0, 0, 0, 1, 0", IF(I67&lt;19,"0, 0, 1, 0, 0",IF(I67&lt;25,"0, 1, 0, 0, 0",IF(I67&lt;27,"1, 0, 0, 0, 0","")))))</f>
+        <f t="shared" ref="K67:K82" si="3">IF(I67&lt;7,"0, 0, 0, 0, 1", IF(I67&lt;13,"0, 0, 0, 1, 0", IF(I67&lt;19,"0, 0, 1, 0, 0",IF(I67&lt;25,"0, 1, 0, 0, 0",IF(I67&lt;27,"1, 0, 0, 0, 0","")))))</f>
         <v>0, 1, 0, 0, 0</v>
       </c>
       <c r="L67" t="str">
-        <f t="shared" ref="L67:L81" si="4">IF(SUMPRODUCT(($A$2:$A$81=A67)*1, ($B$2:$B$81=B67)*1, ($C$2:$C$81=C67)*1,($D$2:$D$81=D67)*1,($E$2:$E$81=E67)*1,($F$2:$F$81=F67)*1,($G$2:$G$81=G67)*1,($H$2:$H$81=H67)*1 ) &gt;1, "duplicates", "no duplicates")</f>
+        <f t="shared" ref="L67:L82" si="4">IF(SUMPRODUCT(($A$2:$A$81=A67)*1, ($B$2:$B$81=B67)*1, ($C$2:$C$81=C67)*1,($D$2:$D$81=D67)*1,($E$2:$E$81=E67)*1,($F$2:$F$81=F67)*1,($G$2:$G$81=G67)*1,($H$2:$H$81=H67)*1 ) &gt;1, "duplicates", "no duplicates")</f>
         <v>no duplicates</v>
       </c>
     </row>
@@ -3011,13 +3044,13 @@
         <v>-3</v>
       </c>
       <c r="C69">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="D69">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E69">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F69">
         <v>-3</v>
@@ -3030,7 +3063,7 @@
       </c>
       <c r="I69">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K69" t="str">
         <f t="shared" si="3"/>
@@ -3052,10 +3085,10 @@
         <v>-3</v>
       </c>
       <c r="D70">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="E70">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="F70">
         <v>0</v>
@@ -3068,7 +3101,7 @@
       </c>
       <c r="I70">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="K70" t="str">
         <f t="shared" si="3"/>
@@ -3087,7 +3120,7 @@
         <v>0</v>
       </c>
       <c r="C71">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -3106,7 +3139,7 @@
       </c>
       <c r="I71">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K71" t="str">
         <f t="shared" si="3"/>
@@ -3119,25 +3152,25 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B72">
         <v>-3</v>
       </c>
       <c r="C72">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="D72">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F72">
         <v>-3</v>
       </c>
       <c r="G72">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="H72">
         <v>-3</v>
@@ -3163,10 +3196,10 @@
         <v>-3</v>
       </c>
       <c r="C73">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="D73">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E73">
         <v>-2</v>
@@ -3178,11 +3211,11 @@
         <v>-3</v>
       </c>
       <c r="H73">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="I73">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K73" t="str">
         <f t="shared" si="3"/>
@@ -3239,7 +3272,7 @@
         <v>-3</v>
       </c>
       <c r="C75">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -3258,7 +3291,7 @@
       </c>
       <c r="I75">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K75" t="str">
         <f t="shared" si="3"/>
@@ -3309,16 +3342,16 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="B77">
         <v>-3</v>
       </c>
       <c r="C77">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="D77">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E77">
         <v>-3</v>
@@ -3334,7 +3367,7 @@
       </c>
       <c r="I77">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K77" t="str">
         <f t="shared" si="3"/>
@@ -3394,7 +3427,7 @@
         <v>0</v>
       </c>
       <c r="D79">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E79">
         <v>0</v>
@@ -3410,7 +3443,7 @@
       </c>
       <c r="I79">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K79" t="str">
         <f t="shared" si="3"/>
@@ -3429,13 +3462,13 @@
         <v>0</v>
       </c>
       <c r="C80">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="D80">
         <v>0</v>
       </c>
       <c r="E80">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F80">
         <v>-1</v>
@@ -3470,7 +3503,7 @@
         <v>-1</v>
       </c>
       <c r="D81">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="E81">
         <v>-3</v>
@@ -3486,7 +3519,7 @@
       </c>
       <c r="I81">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K81" t="str">
         <f t="shared" si="3"/>
@@ -3497,9 +3530,47 @@
         <v>no duplicates</v>
       </c>
     </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>0</v>
+      </c>
+      <c r="B82">
+        <v>-1</v>
+      </c>
+      <c r="C82">
+        <v>-3</v>
+      </c>
+      <c r="D82">
+        <v>-2</v>
+      </c>
+      <c r="E82">
+        <v>-3</v>
+      </c>
+      <c r="F82">
+        <v>-1</v>
+      </c>
+      <c r="G82">
+        <v>-3</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="K82" t="str">
+        <f t="shared" si="3"/>
+        <v>0, 0, 1, 0, 0</v>
+      </c>
+      <c r="L82" t="str">
+        <f t="shared" si="4"/>
+        <v>no duplicates</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:L1">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>